<commit_message>
arreglín en el excel
</commit_message>
<xml_diff>
--- a/libro1.xlsx
+++ b/libro1.xlsx
@@ -411,13 +411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,79 +428,79 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
-      <c r="B4" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="F6" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
-      <c r="I7" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="L8" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="M8" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="N8" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
-      <c r="O9" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="P9" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="R10" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="S10" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="T10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se quitan tags strong
</commit_message>
<xml_diff>
--- a/libro1.xlsx
+++ b/libro1.xlsx
@@ -25,10 +25,10 @@
     <t>valor_ant</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Activos [sinopsis] &lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Activos corrientes [sinopsis] &lt;/strong&gt;</t>
+    <t xml:space="preserve">Activos [sinopsis] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activos corrientes [sinopsis] </t>
   </si>
   <si>
     <t>Efectivo y equivalentes al efectivo</t>
@@ -109,7 +109,7 @@
     <t>Activos corrientes totales</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Activos no corrientes [sinopsis] &lt;/strong&gt;</t>
+    <t xml:space="preserve">Activos no corrientes [sinopsis] </t>
   </si>
   <si>
     <t>Otros activos financieros no corrientes</t>
@@ -208,13 +208,13 @@
     <t>1.546.225.479</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Patrimonio y pasivos [sinopsis] &lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Pasivos [sinopsis] &lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Pasivos corrientes [sinopsis] &lt;/strong&gt;</t>
+    <t xml:space="preserve">Patrimonio y pasivos [sinopsis] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasivos [sinopsis] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasivos corrientes [sinopsis] </t>
   </si>
   <si>
     <t>Otros pasivos financieros corrientes</t>
@@ -295,7 +295,7 @@
     <t>Pasivos corrientes totales</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Pasivos no corrientes [sinopsis] &lt;/strong&gt;</t>
+    <t xml:space="preserve">Pasivos no corrientes [sinopsis] </t>
   </si>
   <si>
     <t>Otros pasivos financieros no corrientes</t>
@@ -376,7 +376,7 @@
     <t>861.973.201</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Patrimonio [sinopsis] &lt;/strong&gt;</t>
+    <t xml:space="preserve">Patrimonio [sinopsis] </t>
   </si>
   <si>
     <t>Capital emitido</t>

</xml_diff>